<commit_message>
MSDS 422, assignment 02
MSDS 422, assignment 02
</commit_message>
<xml_diff>
--- a/MSDS420/Assignment 2/BMoretz_Assignment_02.xlsx
+++ b/MSDS420/Assignment 2/BMoretz_Assignment_02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Notebooks\MSDS420\Assignment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{83D4D4CA-3877-4424-997F-BFCBFABD2D30}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DF3AFD28-7951-499C-8AB9-CDDF29D7072D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26790" windowHeight="13920" xr2:uid="{4FD41947-A134-46F4-9FCB-1C8B9AF75722}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26790" windowHeight="13920" activeTab="2" xr2:uid="{4FD41947-A134-46F4-9FCB-1C8B9AF75722}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="91">
   <si>
     <t>-- 1.) Write a query to count the number of invoices.</t>
   </si>
@@ -51,18 +51,12 @@
     <t>Q2</t>
   </si>
   <si>
-    <t>-- 3.) Generate a listing of all purchases made by customers.</t>
-  </si>
-  <si>
     <t>SELECT</t>
   </si>
   <si>
     <t>C.[CUS_FNAME] || ' ' || C.[CUS_LNAME] AS [Customer Name],</t>
   </si>
   <si>
-    <t>COUNT( [ALL | DISTINCT] ) AS [Orders]</t>
-  </si>
-  <si>
     <t>FROM</t>
   </si>
   <si>
@@ -259,6 +253,57 @@
   </si>
   <si>
     <t>-- including the subtotals for each of the invoice line numbers.</t>
+  </si>
+  <si>
+    <t>I.[INV_NUMBER] AS [Invoice],</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>CustomerCode</t>
+  </si>
+  <si>
+    <t>InvoiceDate</t>
+  </si>
+  <si>
+    <t>LineNumber</t>
+  </si>
+  <si>
+    <t>ProductCode</t>
+  </si>
+  <si>
+    <t>ProductDescription</t>
+  </si>
+  <si>
+    <t>13-Q2/P2</t>
+  </si>
+  <si>
+    <t>23109-HB</t>
+  </si>
+  <si>
+    <t>54778-2T</t>
+  </si>
+  <si>
+    <t>2238/QPD</t>
+  </si>
+  <si>
+    <t>1546-QQ2</t>
+  </si>
+  <si>
+    <t>PVC23DRT</t>
+  </si>
+  <si>
+    <t>SM-18277</t>
+  </si>
+  <si>
+    <t>2232/QTY</t>
+  </si>
+  <si>
+    <t>89-WRE-Q</t>
+  </si>
+  <si>
+    <t>WR3/TT3</t>
   </si>
 </sst>
 </file>
@@ -294,14 +339,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -325,6 +378,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>818607</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>94934</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{164D7C46-6E64-4DCB-AB58-F1096FD28720}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="238125"/>
+          <a:ext cx="4342857" cy="2523809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D3A3C01F-75A7-4B7B-8ECF-8ECFF2C0CB9F}" name="Table13" displayName="Table13" ref="A5:A6" totalsRowShown="0">
   <autoFilter ref="A5:A6" xr:uid="{21785236-2A45-4429-9F76-8AB9E7B37C4D}"/>
@@ -346,22 +448,28 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{EA322510-BF99-4BD2-99D3-2B7CE494A30D}" name="Table3101213" displayName="Table3101213" ref="A17:B22" totalsRowShown="0">
-  <autoFilter ref="A17:B22" xr:uid="{081467CB-7125-4DF8-BE6D-BA8CA5D77E0F}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C263BEE3-8C63-45CE-9111-8D3E12463CDB}" name="Customer Name"/>
-    <tableColumn id="2" xr3:uid="{F2C81227-F27D-48CC-A647-40DAF6A0440B}" name="Orders"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ABC0D67C-4321-44C7-A181-F855A14D56B5}" name="Table1" displayName="Table1" ref="A21:G39" totalsRowShown="0">
+  <autoFilter ref="A21:G39" xr:uid="{B5130106-FE47-44C1-BFB2-EC8DF3A0C15C}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{B3812178-9571-4AA4-B94F-596C53745935}" name="CustomerCode"/>
+    <tableColumn id="2" xr3:uid="{BA1537EB-27F7-4B74-8D8A-C127C8A1990A}" name="Customer Name"/>
+    <tableColumn id="3" xr3:uid="{7FFE946E-2BF9-46C3-A62E-6B65CD44660D}" name="Invoice"/>
+    <tableColumn id="4" xr3:uid="{7CEBEA32-3C36-4FBA-993B-A595FD6E2297}" name="InvoiceDate" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{23513AC9-2D25-48E6-AA8D-A02AF15C67FF}" name="LineNumber" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{FC693DB2-F8F4-4E31-9D82-318E8BD00A81}" name="ProductCode"/>
+    <tableColumn id="7" xr3:uid="{2200D91D-8A9D-4C2D-BF84-C38B349B7FBD}" name="ProductDescription"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{479B0ECE-F3E7-4A3B-B071-59AE0013D76C}" name="Table4" displayName="Table4" ref="B17:C25" totalsRowShown="0">
-  <autoFilter ref="B17:C25" xr:uid="{3D46DFA4-7309-4E20-A313-63BDDDF8CFCF}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{479B0ECE-F3E7-4A3B-B071-59AE0013D76C}" name="Table4" displayName="Table4" ref="B17:D25" totalsRowShown="0">
+  <autoFilter ref="B17:D25" xr:uid="{3D46DFA4-7309-4E20-A313-63BDDDF8CFCF}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8D532494-F489-4724-A0CA-370842B96C8E}" name="Customer Name"/>
-    <tableColumn id="2" xr3:uid="{63518AC0-756A-4EDC-ABEB-0DB80D79D9BD}" name="Balance"/>
+    <tableColumn id="2" xr3:uid="{63518AC0-756A-4EDC-ABEB-0DB80D79D9BD}" name="Invoice"/>
+    <tableColumn id="3" xr3:uid="{17E74B16-5A67-46E1-ADA6-34F304E7AC0E}" name="Balance"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -700,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34D04B9-7F0F-4F9C-AC15-B1DCD9C1DDF7}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,132 +934,487 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D14FB9C-738A-4DE3-9BA2-2350391249C6}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A17:G39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10014</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>1001</v>
+      </c>
+      <c r="D22" s="3">
+        <v>42385</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10014</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>1001</v>
+      </c>
+      <c r="D23" s="3">
+        <v>42385</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10011</v>
+      </c>
+      <c r="B24" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C24">
+        <v>1002</v>
+      </c>
+      <c r="D24" s="3">
+        <v>42385</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10012</v>
+      </c>
+      <c r="B25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C25">
+        <v>1003</v>
+      </c>
+      <c r="D25" s="3">
+        <v>42385</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10012</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>1003</v>
+      </c>
+      <c r="D26" s="3">
+        <v>42385</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10012</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>1003</v>
+      </c>
+      <c r="D27" s="3">
+        <v>42385</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10011</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>1004</v>
+      </c>
+      <c r="D28" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>10011</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>1004</v>
+      </c>
+      <c r="D29" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>10018</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>1005</v>
+      </c>
+      <c r="D30" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10014</v>
+      </c>
+      <c r="B31" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="C31">
+        <v>1006</v>
+      </c>
+      <c r="D31" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>87</v>
+      </c>
+      <c r="G31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10014</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32">
+        <v>1006</v>
+      </c>
+      <c r="D32" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10014</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33">
+        <v>1006</v>
+      </c>
+      <c r="D33" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E33" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="F33" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10014</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34">
+        <v>1006</v>
+      </c>
+      <c r="D34" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>10015</v>
+      </c>
+      <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="C35">
+        <v>1007</v>
+      </c>
+      <c r="D35" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
+      <c r="F35" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>10015</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36">
+        <v>1007</v>
+      </c>
+      <c r="D36" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E36" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
+      <c r="F36" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>10011</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <v>1008</v>
+      </c>
+      <c r="D37" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E37" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
+      <c r="F37" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>10011</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38">
+        <v>1008</v>
+      </c>
+      <c r="D38" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>10011</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39">
+        <v>1008</v>
+      </c>
+      <c r="D39" s="3">
+        <v>42386</v>
+      </c>
+      <c r="E39" s="2">
+        <v>3</v>
+      </c>
+      <c r="F39" t="s">
+        <v>82</v>
+      </c>
+      <c r="G39" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E753968-ED52-4762-8C83-C8DDDBB2AF2A}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,138 +1425,175 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>1001</v>
+      </c>
+      <c r="D18">
+        <v>24.94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C19">
+        <v>1002</v>
+      </c>
+      <c r="D19">
+        <v>9.98</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>1003</v>
+      </c>
+      <c r="D20">
+        <v>153.85</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>1004</v>
+      </c>
+      <c r="D21">
+        <v>34.869999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C18">
-        <v>24.94</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="C22">
+        <v>1005</v>
+      </c>
+      <c r="D22">
+        <v>70.44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="C19">
-        <v>9.98</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C23">
+        <v>1006</v>
+      </c>
+      <c r="D23">
+        <v>397.83</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="C20">
-        <v>153.85</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21">
-        <v>34.869999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22">
-        <v>70.44</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23">
-        <v>397.83</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
       <c r="C24">
+        <v>1007</v>
+      </c>
+      <c r="D24">
         <v>34.97</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25">
+        <v>1008</v>
+      </c>
+      <c r="D25">
         <v>399.15</v>
       </c>
     </row>
@@ -1121,83 +1621,83 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -1208,7 +1708,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1219,7 +1719,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1230,7 +1730,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1241,7 +1741,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1273,87 +1773,87 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B15:B19">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1379,58 +1879,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>879.92</v>
@@ -1441,7 +1941,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>479.68</v>
@@ -1452,7 +1952,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>314.82</v>
@@ -1463,7 +1963,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15">
         <v>599.25</v>
@@ -1474,7 +1974,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>1011.77</v>
@@ -1485,7 +1985,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17">
         <v>879.36</v>
@@ -1496,7 +1996,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C18">
         <v>599.22</v>
@@ -1507,7 +2007,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19">
         <v>467.4</v>
@@ -1518,7 +2018,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20">
         <v>228.85</v>
@@ -1529,7 +2029,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21">
         <v>115.2</v>
@@ -1540,7 +2040,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22">
         <v>214.57</v>
@@ -1551,7 +2051,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23">
         <v>2826.89</v>
@@ -1562,7 +2062,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24">
         <v>1103.56</v>
@@ -1573,7 +2073,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25">
         <v>1202.28</v>
@@ -1584,7 +2084,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26">
         <v>2002.6499999999901</v>
@@ -1595,7 +2095,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C27">
         <v>2159.1</v>

</xml_diff>